<commit_message>
Organized final simper output
</commit_message>
<xml_diff>
--- a/simper.xlsx
+++ b/simper.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Cecum_Microbes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{591B5A65-61C8-47ED-9A09-23E32EF02106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A951A8-5279-4EDF-B993-BBEAEF98E55D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6336" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simper" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="118">
   <si>
     <t>Comparison</t>
   </si>
@@ -358,13 +358,31 @@
   </si>
   <si>
     <t>Firmicutes - Clostridia - Clostridiales - Lachnospiraceae - Roseburia</t>
+  </si>
+  <si>
+    <t>In all Summer_Wild (enriched)</t>
+  </si>
+  <si>
+    <t>In Summer_Wild (enriched in all comp except Spring)</t>
+  </si>
+  <si>
+    <t>In all Summer_Lab (enriched)</t>
+  </si>
+  <si>
+    <t>In spring (enriched)</t>
+  </si>
+  <si>
+    <t>In torpor (enriched)</t>
+  </si>
+  <si>
+    <t>In Summer_Lab (enriched)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,8 +517,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,6 +710,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -847,11 +901,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1206,7 +1269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10219,17 +10282,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -10267,984 +10331,1078 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>1.1295018093398E-2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="8">
         <v>1.01364918243408E-4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="8">
         <v>3.33199339917379E-3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="8">
         <v>1.9247791674173301E-2</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="8">
         <v>2.82641262947637E-2</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="8">
         <v>0</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="8">
         <v>1.3915708282640001E-2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>1.0412479372418099E-4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="8">
         <v>3.33199339917379E-3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="8">
         <v>2.3789103765922401E-2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="8">
         <v>1.80802408553861E-2</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="8">
         <v>0</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="8">
         <v>1.1552670847151E-2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>1.0412479372418099E-4</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="8">
         <v>3.33199339917379E-3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="8">
         <v>1.9694669210578102E-2</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="8">
         <v>2.5925640306717099E-2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="8">
         <v>0</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>2.7616702700022401E-2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>8.8487129808296496E-4</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>1.33251207240729E-2</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>3.7080806013536899E-4</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>5.7349259814279798E-4</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>4.7400311518731697E-2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>5.8102965390865902E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="11">
         <v>1.44520780781418E-2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="11">
         <v>2.9697533142072998E-3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="11">
         <v>2.71520303013239E-2</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="11">
         <v>2.4657890514991902E-2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="11">
         <v>3.7529057748907198E-2</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="11">
         <v>0</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
         <v>1.0809407165093999E-2</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>1.79431037512558E-4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="8">
         <v>4.7285345245315601E-3</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="8">
         <v>1.9247791674173301E-2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="8">
         <v>2.82641262947637E-2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="8">
         <v>0</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="8">
         <v>1.1055976857280001E-2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>1.8470837986451401E-4</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="8">
         <v>4.7285345245315601E-3</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="8">
         <v>1.9694669210578102E-2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="8">
         <v>2.5925640306717099E-2</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="8">
         <v>0</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <v>1.3310759684281E-2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>3.3619350474802602E-4</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="8">
         <v>5.7377024810329798E-3</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="8">
         <v>2.3789103765922401E-2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="8">
         <v>1.80802408553861E-2</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="9">
         <v>1.1741223435482E-5</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="9">
         <v>3.71290085730701E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>1.1707414934041999E-2</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="10">
         <v>1.13809558467493E-3</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="10">
         <v>1.4567623483839101E-2</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="10">
         <v>1.10159518614379E-3</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="10">
         <v>6.3168703798115503E-4</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="10">
         <v>2.1943457030843001E-2</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="10">
         <v>1.9729309857584899E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
         <v>1.3830712972158999E-2</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>4.3735451621768496E-3</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="8">
         <v>3.6117018113460402E-2</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="8">
         <v>2.4657890514991902E-2</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="8">
         <v>3.7529057748907198E-2</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="8">
         <v>0</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="8">
         <v>1.0771216365661E-2</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="9">
         <v>3.3071975235261398E-5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="8">
         <v>2.1666724230667601E-3</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="8">
         <v>1.9247791674173301E-2</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="8">
         <v>2.82641262947637E-2</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="8">
         <v>0</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <v>1.3270373913103E-2</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="9">
         <v>3.3854256610418202E-5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="8">
         <v>2.1666724230667601E-3</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="8">
         <v>2.3789103765922401E-2</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="8">
         <v>1.80802408553861E-2</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="8">
         <v>0</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="8">
         <v>1.1016920660732E-2</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="9">
         <v>3.3854256610418202E-5</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="8">
         <v>2.1666724230667601E-3</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="8">
         <v>1.9694669210578102E-2</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="8">
         <v>2.5925640306717099E-2</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="8">
         <v>0</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="8">
         <v>1.3781869316281999E-2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
         <v>1.38873912507698E-3</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="8">
         <v>1.61598734554412E-2</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="8">
         <v>2.4657890514991902E-2</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="8">
         <v>3.7529057748907198E-2</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="8">
         <v>0</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="12">
         <v>1.1124093432768999E-2</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="12">
         <v>1.38873912507698E-3</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="12">
         <v>1.61598734554412E-2</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="12">
         <v>1.9901281365748699E-2</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="12">
         <v>1.89649089836606E-2</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="12">
         <v>0</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="8">
         <v>1.0561291256562E-2</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <v>1.0679544323162901E-3</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="8">
         <v>1.4567623483839101E-2</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="8">
         <v>1.9247791674173301E-2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="8">
         <v>2.82641262947637E-2</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="8">
         <v>0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="8">
         <v>1.0802199463477999E-2</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <v>1.1088549089766999E-3</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="8">
         <v>1.4567623483839101E-2</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="8">
         <v>1.9694669210578102E-2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="8">
         <v>2.5925640306717099E-2</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="8">
         <v>0</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="2" t="s">
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="8">
         <v>1.3002479854329001E-2</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="8">
         <v>1.6020006947992801E-3</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="8">
         <v>1.7830964255157199E-2</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="8">
         <v>2.3789103765922401E-2</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="8">
         <v>1.80802408553861E-2</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="9">
         <v>1.66267624368183E-5</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="9">
         <v>4.39902785159715E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <v>3.9497742123962599E-2</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>3.2745584338682901E-3</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="6">
         <v>2.8906446864492501E-2</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="6">
         <v>1.3657816596969799E-4</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="6">
         <v>1.3556671056483201E-4</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="6">
         <v>7.1894686722130896E-2</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="6">
         <v>8.7797190858769497E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <v>2.7725198376336E-2</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="5">
         <v>5.4996183839537499E-5</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="4">
         <v>2.81580461258432E-3</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="4">
         <v>4.7400311518731697E-2</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="4">
         <v>5.8102965390865902E-2</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="5">
         <v>1.1738466956215501E-5</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="5">
         <v>3.7120291820264998E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="30" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="10">
         <v>1.2175267310142001E-2</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="10">
         <v>6.6566791015996898E-4</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="10">
         <v>1.06506865625595E-2</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="10">
         <v>2.3979079223339899E-3</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="10">
         <v>6.21178943485696E-3</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="10">
         <v>2.1943457030843001E-2</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="10">
         <v>1.9729309857584899E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="2" t="s">
+    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <v>1.607916424789E-2</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="4">
         <v>2.8778055189991698E-3</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="4">
         <v>2.71520303013239E-2</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="4">
         <v>2.7592525412283402E-2</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="4">
         <v>5.7482602533928999E-2</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="5">
         <v>3.52675713137514E-5</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="5">
         <v>5.67874682410705E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <v>2.7435485687436999E-2</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="5">
         <v>1.32442449026243E-5</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="4">
         <v>2.1666724230667601E-3</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="4">
         <v>4.7400311518731697E-2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="4">
         <v>5.8102965390865902E-2</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="4">
         <v>1.54017976140565E-4</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="4">
         <v>5.2110769374237099E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="2" t="s">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <v>1.5968772078577002E-2</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="4">
         <v>2.2587284430861901E-4</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="4">
         <v>5.2566771039096799E-3</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="4">
         <v>2.7592525412283402E-2</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="4">
         <v>5.7482602533928999E-2</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="5">
         <v>9.0168886324085006E-6</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="5">
         <v>3.2510854309297199E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="12">
         <v>0.121018150057878</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="12">
         <v>2.7225075192438401E-3</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="12">
         <v>2.6806227881785501E-2</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="12">
         <v>3.2997999598677798E-3</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="12">
         <v>6.4097516690018496E-3</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="12">
         <v>0.21053585852432</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="12">
         <v>0.24566793432419201</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="2" t="s">
+    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="4">
         <v>2.8218195754358001E-2</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="4">
         <v>3.2794821051791403E-4</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="4">
         <v>5.7377024810329798E-3</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="4">
         <v>4.7400311518731697E-2</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="4">
         <v>5.8102965390865902E-2</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="4">
         <v>0</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="2" t="s">
+    <row r="43" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="6">
         <v>4.0454600996608997E-2</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="6">
         <v>3.1058329336570702E-4</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="6">
         <v>5.7377024810329798E-3</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="7">
         <v>3.5132580336041499E-5</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="7">
         <v>7.88952172593031E-5</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="6">
         <v>7.1894686722130896E-2</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="6">
         <v>8.7797190858769497E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="2" t="s">
+    <row r="45" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="6">
         <v>4.0473052233953997E-2</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="6">
         <v>2.68998403609918E-4</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="6">
         <v>5.7377024810329798E-3</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="7">
         <v>9.9835804737582299E-5</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="6">
         <v>1.0605337368479E-4</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="6">
         <v>7.1894686722130896E-2</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="6">
         <v>8.7797190858769497E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -11253,10 +11411,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>